<commit_message>
Cambios a documentación Octubre 4
</commit_message>
<xml_diff>
--- a/Enterprise architect/DiccionarioDeDatos.xlsx
+++ b/Enterprise architect/DiccionarioDeDatos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Transforma2017\Transforma\Grupo Metropolitano\Cotizaciones\2017\11 Implementación de conciliación\Diccionario de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Proyectos\Conciliacion Bancaria GM\Enterprise architect\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -492,9 +492,6 @@
     <t>Mes de la creación de la conciliación</t>
   </si>
   <si>
-    <t>Consecutivo por mes, año, sucursal de la conciliacióm</t>
-  </si>
-  <si>
     <t>Llave foranea de la tabla TableDestinoDetalle que nos indica el archivo externo de la conciliación</t>
   </si>
   <si>
@@ -1054,12 +1051,15 @@
   </si>
   <si>
     <t>Indica los usuarios registrado en el sistema</t>
+  </si>
+  <si>
+    <t>Consecutivo por mes, año, sucursal de la conciliación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1569,7 +1569,7 @@
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -1872,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,13 +1886,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>149</v>
@@ -1903,13 +1903,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1917,13 +1917,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1939,7 +1939,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,7 +1955,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1971,13 +1971,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1993,7 +1993,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2017,13 +2017,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2063,7 +2063,7 @@
         <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2071,7 +2071,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2079,7 +2079,7 @@
         <v>16</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>23</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,7 +2095,7 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2103,7 +2103,7 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2111,7 +2111,7 @@
         <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
         <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2135,7 +2135,7 @@
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2143,7 +2143,7 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2159,7 +2159,7 @@
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2167,13 +2167,13 @@
         <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C32" t="s">
         <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2181,7 +2181,7 @@
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2189,7 +2189,7 @@
         <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2205,7 +2205,7 @@
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>28</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2221,7 +2221,7 @@
         <v>26</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,7 @@
         <v>29</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
         <v>27</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2245,13 +2245,13 @@
         <v>30</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C41" t="s">
         <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,7 +2259,7 @@
         <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2267,7 +2267,7 @@
         <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2275,7 +2275,7 @@
         <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2291,7 +2291,7 @@
         <v>34</v>
       </c>
       <c r="D46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
         <v>41</v>
       </c>
       <c r="D47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
@@ -2315,7 +2315,7 @@
         <v>11</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
@@ -2323,7 +2323,7 @@
         <v>23</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
@@ -2331,7 +2331,7 @@
         <v>16</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
@@ -2339,7 +2339,7 @@
         <v>35</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
@@ -2347,7 +2347,7 @@
         <v>42</v>
       </c>
       <c r="D53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
@@ -2355,7 +2355,7 @@
         <v>38</v>
       </c>
       <c r="D54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
@@ -2363,7 +2363,7 @@
         <v>37</v>
       </c>
       <c r="D55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
@@ -2371,7 +2371,7 @@
         <v>36</v>
       </c>
       <c r="D56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
@@ -2379,7 +2379,7 @@
         <v>40</v>
       </c>
       <c r="D57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
@@ -2387,7 +2387,7 @@
         <v>33</v>
       </c>
       <c r="D58" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
         <v>32</v>
       </c>
       <c r="D60" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
@@ -2411,7 +2411,7 @@
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
@@ -2427,7 +2427,7 @@
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
@@ -2435,7 +2435,7 @@
         <v>31</v>
       </c>
       <c r="D64" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2443,7 +2443,7 @@
         <v>39</v>
       </c>
       <c r="D65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2451,13 +2451,13 @@
         <v>43</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C66" t="s">
         <v>22</v>
       </c>
       <c r="D66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2465,7 +2465,7 @@
         <v>12</v>
       </c>
       <c r="D67" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2473,7 +2473,7 @@
         <v>24</v>
       </c>
       <c r="D68" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2481,7 +2481,7 @@
         <v>17</v>
       </c>
       <c r="D69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2489,7 +2489,7 @@
         <v>14</v>
       </c>
       <c r="D70" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,7 +2497,7 @@
         <v>34</v>
       </c>
       <c r="D71" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2505,7 +2505,7 @@
         <v>51</v>
       </c>
       <c r="D72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2513,7 +2513,7 @@
         <v>52</v>
       </c>
       <c r="D73" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2521,7 +2521,7 @@
         <v>47</v>
       </c>
       <c r="D74" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>21</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2537,7 +2537,7 @@
         <v>11</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2545,7 +2545,7 @@
         <v>23</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2553,7 +2553,7 @@
         <v>16</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>35</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2569,7 +2569,7 @@
         <v>42</v>
       </c>
       <c r="D80" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
@@ -2577,7 +2577,7 @@
         <v>46</v>
       </c>
       <c r="D81" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
         <v>45</v>
       </c>
       <c r="D82" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
@@ -2593,7 +2593,7 @@
         <v>49</v>
       </c>
       <c r="D83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
@@ -2601,7 +2601,7 @@
         <v>44</v>
       </c>
       <c r="D84" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
@@ -2609,7 +2609,7 @@
         <v>38</v>
       </c>
       <c r="D85" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.25">
@@ -2617,7 +2617,7 @@
         <v>37</v>
       </c>
       <c r="D86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.25">
@@ -2625,7 +2625,7 @@
         <v>36</v>
       </c>
       <c r="D87" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.25">
@@ -2633,7 +2633,7 @@
         <v>40</v>
       </c>
       <c r="D88" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.25">
@@ -2641,7 +2641,7 @@
         <v>33</v>
       </c>
       <c r="D89" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.25">
@@ -2649,7 +2649,7 @@
         <v>13</v>
       </c>
       <c r="D90" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.25">
@@ -2657,7 +2657,7 @@
         <v>32</v>
       </c>
       <c r="D91" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.25">
@@ -2665,7 +2665,7 @@
         <v>48</v>
       </c>
       <c r="D92" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
         <v>50</v>
       </c>
       <c r="D93" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.25">
@@ -2681,7 +2681,7 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.25">
@@ -2697,7 +2697,7 @@
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2705,7 +2705,7 @@
         <v>31</v>
       </c>
       <c r="D97" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2713,7 +2713,7 @@
         <v>39</v>
       </c>
       <c r="D98" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2721,13 +2721,13 @@
         <v>53</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C99" t="s">
         <v>22</v>
       </c>
       <c r="D99" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2735,7 +2735,7 @@
         <v>12</v>
       </c>
       <c r="D100" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>24</v>
       </c>
       <c r="D101" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2759,7 +2759,7 @@
         <v>17</v>
       </c>
       <c r="D103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2767,7 +2767,7 @@
         <v>34</v>
       </c>
       <c r="D104" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2775,7 +2775,7 @@
         <v>28</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2783,7 +2783,7 @@
         <v>26</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
         <v>29</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2799,7 +2799,7 @@
         <v>27</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2807,7 +2807,7 @@
         <v>54</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2815,7 +2815,7 @@
         <v>21</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2823,7 +2823,7 @@
         <v>11</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2831,7 +2831,7 @@
         <v>23</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="113" spans="3:4" x14ac:dyDescent="0.25">
@@ -2839,7 +2839,7 @@
         <v>16</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="114" spans="3:4" x14ac:dyDescent="0.25">
@@ -2847,7 +2847,7 @@
         <v>35</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="115" spans="3:4" x14ac:dyDescent="0.25">
@@ -2855,7 +2855,7 @@
         <v>42</v>
       </c>
       <c r="D115" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="116" spans="3:4" x14ac:dyDescent="0.25">
@@ -2863,7 +2863,7 @@
         <v>38</v>
       </c>
       <c r="D116" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="117" spans="3:4" x14ac:dyDescent="0.25">
@@ -2871,7 +2871,7 @@
         <v>55</v>
       </c>
       <c r="D117" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" spans="3:4" x14ac:dyDescent="0.25">
@@ -2879,7 +2879,7 @@
         <v>37</v>
       </c>
       <c r="D118" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="119" spans="3:4" x14ac:dyDescent="0.25">
@@ -2887,7 +2887,7 @@
         <v>36</v>
       </c>
       <c r="D119" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="120" spans="3:4" x14ac:dyDescent="0.25">
@@ -2895,7 +2895,7 @@
         <v>40</v>
       </c>
       <c r="D120" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="121" spans="3:4" x14ac:dyDescent="0.25">
@@ -2903,7 +2903,7 @@
         <v>33</v>
       </c>
       <c r="D121" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="122" spans="3:4" x14ac:dyDescent="0.25">
@@ -2911,7 +2911,7 @@
         <v>13</v>
       </c>
       <c r="D122" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="123" spans="3:4" x14ac:dyDescent="0.25">
@@ -2919,7 +2919,7 @@
         <v>48</v>
       </c>
       <c r="D123" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="124" spans="3:4" x14ac:dyDescent="0.25">
@@ -2927,7 +2927,7 @@
         <v>50</v>
       </c>
       <c r="D124" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="125" spans="3:4" x14ac:dyDescent="0.25">
@@ -2935,7 +2935,7 @@
         <v>2</v>
       </c>
       <c r="D125" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="126" spans="3:4" x14ac:dyDescent="0.25">
@@ -2951,7 +2951,7 @@
         <v>5</v>
       </c>
       <c r="D127" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="128" spans="3:4" x14ac:dyDescent="0.25">
@@ -2959,7 +2959,7 @@
         <v>31</v>
       </c>
       <c r="D128" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -2967,7 +2967,7 @@
         <v>39</v>
       </c>
       <c r="D129" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2975,13 +2975,13 @@
         <v>56</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C130" t="s">
         <v>56</v>
       </c>
       <c r="D130" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -2989,7 +2989,7 @@
         <v>60</v>
       </c>
       <c r="D131" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2997,7 +2997,7 @@
         <v>61</v>
       </c>
       <c r="D132" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3013,7 +3013,7 @@
         <v>58</v>
       </c>
       <c r="D134" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3021,7 +3021,7 @@
         <v>59</v>
       </c>
       <c r="D135" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3029,13 +3029,13 @@
         <v>62</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C136" t="s">
         <v>56</v>
       </c>
       <c r="D136" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3043,7 +3043,7 @@
         <v>20</v>
       </c>
       <c r="D137" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3067,7 +3067,7 @@
         <v>63</v>
       </c>
       <c r="D140" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3075,7 +3075,7 @@
         <v>64</v>
       </c>
       <c r="D141" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3083,13 +3083,13 @@
         <v>67</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C142" t="s">
         <v>67</v>
       </c>
       <c r="D142" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3097,7 +3097,7 @@
         <v>72</v>
       </c>
       <c r="D143" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
         <v>68</v>
       </c>
       <c r="D144" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3113,7 +3113,7 @@
         <v>70</v>
       </c>
       <c r="D145" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3121,7 +3121,7 @@
         <v>74</v>
       </c>
       <c r="D146" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3129,7 +3129,7 @@
         <v>75</v>
       </c>
       <c r="D147" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3137,7 +3137,7 @@
         <v>73</v>
       </c>
       <c r="D148" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3145,7 +3145,7 @@
         <v>69</v>
       </c>
       <c r="D149" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3153,7 +3153,7 @@
         <v>71</v>
       </c>
       <c r="D150" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3161,7 +3161,7 @@
         <v>77</v>
       </c>
       <c r="D151" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3169,7 +3169,7 @@
         <v>76</v>
       </c>
       <c r="D152" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3185,7 +3185,7 @@
         <v>9</v>
       </c>
       <c r="D154" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3201,13 +3201,13 @@
         <v>78</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C156" t="s">
         <v>80</v>
       </c>
       <c r="D156" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3215,7 +3215,7 @@
         <v>82</v>
       </c>
       <c r="D157" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3223,7 +3223,7 @@
         <v>79</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>81</v>
       </c>
       <c r="D159" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3239,13 +3239,13 @@
         <v>83</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C160" t="s">
         <v>83</v>
       </c>
       <c r="D160" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3253,7 +3253,7 @@
         <v>89</v>
       </c>
       <c r="D161" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3261,7 +3261,7 @@
         <v>85</v>
       </c>
       <c r="D162" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3269,7 +3269,7 @@
         <v>87</v>
       </c>
       <c r="D163" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -3277,7 +3277,7 @@
         <v>79</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -3301,7 +3301,7 @@
         <v>9</v>
       </c>
       <c r="D167" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -3309,7 +3309,7 @@
         <v>86</v>
       </c>
       <c r="D168" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -3317,7 +3317,7 @@
         <v>84</v>
       </c>
       <c r="D169" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3325,7 +3325,7 @@
         <v>80</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3333,7 +3333,7 @@
         <v>82</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3341,7 +3341,7 @@
         <v>88</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3349,13 +3349,13 @@
         <v>41</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C173" t="s">
         <v>41</v>
       </c>
       <c r="D173" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3363,13 +3363,13 @@
         <v>90</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C174" t="s">
         <v>66</v>
       </c>
       <c r="D174" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -3377,7 +3377,7 @@
         <v>65</v>
       </c>
       <c r="D175" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -3385,7 +3385,7 @@
         <v>33</v>
       </c>
       <c r="D176" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -3393,7 +3393,7 @@
         <v>91</v>
       </c>
       <c r="D177" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
         <v>94</v>
       </c>
       <c r="D178" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>56</v>
       </c>
       <c r="D179" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -3417,7 +3417,7 @@
         <v>93</v>
       </c>
       <c r="D180" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3425,7 +3425,7 @@
         <v>92</v>
       </c>
       <c r="D181" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -3433,7 +3433,7 @@
         <v>2</v>
       </c>
       <c r="D182" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -3449,13 +3449,13 @@
         <v>40</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C184" t="s">
         <v>40</v>
       </c>
       <c r="D184" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -3463,7 +3463,7 @@
         <v>5</v>
       </c>
       <c r="D185" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -3471,13 +3471,13 @@
         <v>95</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C186" t="s">
         <v>95</v>
       </c>
       <c r="D186" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -3485,7 +3485,7 @@
         <v>5</v>
       </c>
       <c r="D187" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -3493,13 +3493,13 @@
         <v>96</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C188" t="s">
         <v>20</v>
       </c>
       <c r="D188" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -3507,7 +3507,7 @@
         <v>89</v>
       </c>
       <c r="D189" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
         <v>96</v>
       </c>
       <c r="D190" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -3523,7 +3523,7 @@
         <v>99</v>
       </c>
       <c r="D191" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -3531,7 +3531,7 @@
         <v>85</v>
       </c>
       <c r="D192" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -3539,7 +3539,7 @@
         <v>98</v>
       </c>
       <c r="D193" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -3547,7 +3547,7 @@
         <v>100</v>
       </c>
       <c r="D194" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -3555,7 +3555,7 @@
         <v>97</v>
       </c>
       <c r="D195" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3563,13 +3563,13 @@
         <v>101</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C196" t="s">
         <v>20</v>
       </c>
       <c r="D196" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -3577,7 +3577,7 @@
         <v>89</v>
       </c>
       <c r="D197" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -3585,7 +3585,7 @@
         <v>96</v>
       </c>
       <c r="D198" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -3593,7 +3593,7 @@
         <v>102</v>
       </c>
       <c r="D199" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -3601,7 +3601,7 @@
         <v>104</v>
       </c>
       <c r="D200" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -3609,7 +3609,7 @@
         <v>80</v>
       </c>
       <c r="D201" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -3617,7 +3617,7 @@
         <v>82</v>
       </c>
       <c r="D202" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -3625,7 +3625,7 @@
         <v>1</v>
       </c>
       <c r="D203" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -3633,7 +3633,7 @@
         <v>103</v>
       </c>
       <c r="D204" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -3641,13 +3641,13 @@
         <v>105</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C205" t="s">
         <v>20</v>
       </c>
       <c r="D205" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -3655,7 +3655,7 @@
         <v>89</v>
       </c>
       <c r="D206" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -3663,7 +3663,7 @@
         <v>96</v>
       </c>
       <c r="D207" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -3671,7 +3671,7 @@
         <v>102</v>
       </c>
       <c r="D208" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -3679,7 +3679,7 @@
         <v>83</v>
       </c>
       <c r="D209" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -3687,7 +3687,7 @@
         <v>106</v>
       </c>
       <c r="D210" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -3695,7 +3695,7 @@
         <v>107</v>
       </c>
       <c r="D211" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -3703,13 +3703,13 @@
         <v>15</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C212" t="s">
         <v>15</v>
       </c>
       <c r="D212" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -3717,7 +3717,7 @@
         <v>5</v>
       </c>
       <c r="D213" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -3725,7 +3725,7 @@
         <v>2</v>
       </c>
       <c r="D214" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -3749,7 +3749,7 @@
         <v>109</v>
       </c>
       <c r="D217" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -3757,7 +3757,7 @@
         <v>110</v>
       </c>
       <c r="D218" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -3765,7 +3765,7 @@
         <v>111</v>
       </c>
       <c r="D219" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -3773,7 +3773,7 @@
         <v>112</v>
       </c>
       <c r="D220" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -3781,7 +3781,7 @@
         <v>113</v>
       </c>
       <c r="D221" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -3789,7 +3789,7 @@
         <v>114</v>
       </c>
       <c r="D222" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,7 +3797,7 @@
         <v>108</v>
       </c>
       <c r="D223" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -3805,13 +3805,13 @@
         <v>115</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C224" t="s">
         <v>15</v>
       </c>
       <c r="D224" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -3819,7 +3819,7 @@
         <v>33</v>
       </c>
       <c r="D225" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -3827,13 +3827,13 @@
         <v>116</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C226" t="s">
         <v>15</v>
       </c>
       <c r="D226" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -3841,7 +3841,7 @@
         <v>2</v>
       </c>
       <c r="D227" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -3849,7 +3849,7 @@
         <v>117</v>
       </c>
       <c r="D228" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3857,13 +3857,13 @@
         <v>118</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C229" t="s">
         <v>118</v>
       </c>
       <c r="D229" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -3871,7 +3871,7 @@
         <v>5</v>
       </c>
       <c r="D230" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -3879,7 +3879,7 @@
         <v>85</v>
       </c>
       <c r="D231" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -3887,7 +3887,7 @@
         <v>119</v>
       </c>
       <c r="D232" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -3903,13 +3903,13 @@
         <v>120</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C234" t="s">
         <v>118</v>
       </c>
       <c r="D234" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -3917,7 +3917,7 @@
         <v>20</v>
       </c>
       <c r="D235" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -3925,13 +3925,13 @@
         <v>48</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C236" t="s">
         <v>48</v>
       </c>
       <c r="D236" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -3939,7 +3939,7 @@
         <v>5</v>
       </c>
       <c r="D237" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -3955,13 +3955,13 @@
         <v>47</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C239" t="s">
         <v>47</v>
       </c>
       <c r="D239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -3969,7 +3969,7 @@
         <v>51</v>
       </c>
       <c r="D240" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -3977,7 +3977,7 @@
         <v>52</v>
       </c>
       <c r="D241" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -3985,13 +3985,13 @@
         <v>121</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C242" t="s">
         <v>121</v>
       </c>
       <c r="D242" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -4007,13 +4007,13 @@
         <v>33</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C244" t="s">
         <v>33</v>
       </c>
       <c r="D244" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -4021,7 +4021,7 @@
         <v>5</v>
       </c>
       <c r="D245" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -4029,7 +4029,7 @@
         <v>2</v>
       </c>
       <c r="D246" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -4053,7 +4053,7 @@
         <v>91</v>
       </c>
       <c r="D249" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -4061,7 +4061,7 @@
         <v>122</v>
       </c>
       <c r="D250" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>123</v>
       </c>
       <c r="D251" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -4077,7 +4077,7 @@
         <v>124</v>
       </c>
       <c r="D252" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4085,13 +4085,13 @@
         <v>13</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C253" t="s">
         <v>13</v>
       </c>
       <c r="D253" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -4099,7 +4099,7 @@
         <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -4123,7 +4123,7 @@
         <v>125</v>
       </c>
       <c r="D257" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4131,13 +4131,13 @@
         <v>32</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C258" t="s">
         <v>32</v>
       </c>
       <c r="D258" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -4145,13 +4145,13 @@
         <v>98</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C259" t="s">
         <v>98</v>
       </c>
       <c r="D259" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -4159,7 +4159,7 @@
         <v>5</v>
       </c>
       <c r="D260" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -4167,7 +4167,7 @@
         <v>127</v>
       </c>
       <c r="D261" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -4175,7 +4175,7 @@
         <v>126</v>
       </c>
       <c r="D262" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
@@ -4183,7 +4183,7 @@
         <v>59</v>
       </c>
       <c r="D263" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
         <v>56</v>
       </c>
       <c r="D264" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4199,13 +4199,13 @@
         <v>80</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C265" t="s">
         <v>56</v>
       </c>
       <c r="D265" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -4213,7 +4213,7 @@
         <v>98</v>
       </c>
       <c r="D266" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>66</v>
       </c>
       <c r="D267" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -4229,7 +4229,7 @@
         <v>128</v>
       </c>
       <c r="D268" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -4237,7 +4237,7 @@
         <v>20</v>
       </c>
       <c r="D269" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -4245,7 +4245,7 @@
         <v>85</v>
       </c>
       <c r="D270" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
         <v>95</v>
       </c>
       <c r="D271" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -4261,7 +4261,7 @@
         <v>18</v>
       </c>
       <c r="D272" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -4269,7 +4269,7 @@
         <v>19</v>
       </c>
       <c r="D273" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -4277,7 +4277,7 @@
         <v>13</v>
       </c>
       <c r="D274" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -4285,7 +4285,7 @@
         <v>2</v>
       </c>
       <c r="D275" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
@@ -4301,13 +4301,13 @@
         <v>129</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C277" t="s">
         <v>56</v>
       </c>
       <c r="D277" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
@@ -4315,7 +4315,7 @@
         <v>98</v>
       </c>
       <c r="D278" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -4323,7 +4323,7 @@
         <v>66</v>
       </c>
       <c r="D279" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -4331,7 +4331,7 @@
         <v>128</v>
       </c>
       <c r="D280" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -4339,7 +4339,7 @@
         <v>102</v>
       </c>
       <c r="D281" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -4347,7 +4347,7 @@
         <v>142</v>
       </c>
       <c r="D282" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -4355,7 +4355,7 @@
         <v>138</v>
       </c>
       <c r="D283" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -4363,7 +4363,7 @@
         <v>139</v>
       </c>
       <c r="D284" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
         <v>134</v>
       </c>
       <c r="D285" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -4379,7 +4379,7 @@
         <v>5</v>
       </c>
       <c r="D286" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
@@ -4387,7 +4387,7 @@
         <v>130</v>
       </c>
       <c r="D287" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
@@ -4395,7 +4395,7 @@
         <v>131</v>
       </c>
       <c r="D288" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="289" spans="3:4" x14ac:dyDescent="0.25">
@@ -4403,7 +4403,7 @@
         <v>140</v>
       </c>
       <c r="D289" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="290" spans="3:4" x14ac:dyDescent="0.25">
@@ -4411,7 +4411,7 @@
         <v>133</v>
       </c>
       <c r="D290" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="291" spans="3:4" x14ac:dyDescent="0.25">
@@ -4419,7 +4419,7 @@
         <v>63</v>
       </c>
       <c r="D291" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="292" spans="3:4" x14ac:dyDescent="0.25">
@@ -4427,7 +4427,7 @@
         <v>64</v>
       </c>
       <c r="D292" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="293" spans="3:4" x14ac:dyDescent="0.25">
@@ -4443,7 +4443,7 @@
         <v>141</v>
       </c>
       <c r="D294" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="295" spans="3:4" x14ac:dyDescent="0.25">
@@ -4451,7 +4451,7 @@
         <v>145</v>
       </c>
       <c r="D295" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="296" spans="3:4" x14ac:dyDescent="0.25">
@@ -4459,7 +4459,7 @@
         <v>132</v>
       </c>
       <c r="D296" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="297" spans="3:4" x14ac:dyDescent="0.25">
@@ -4467,7 +4467,7 @@
         <v>136</v>
       </c>
       <c r="D297" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="298" spans="3:4" x14ac:dyDescent="0.25">
@@ -4475,7 +4475,7 @@
         <v>144</v>
       </c>
       <c r="D298" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="299" spans="3:4" x14ac:dyDescent="0.25">
@@ -4483,7 +4483,7 @@
         <v>42</v>
       </c>
       <c r="D299" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="300" spans="3:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4491,7 @@
         <v>135</v>
       </c>
       <c r="D300" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="301" spans="3:4" x14ac:dyDescent="0.25">
@@ -4499,7 +4499,7 @@
         <v>0</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="302" spans="3:4" x14ac:dyDescent="0.25">
@@ -4507,7 +4507,7 @@
         <v>33</v>
       </c>
       <c r="D302" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="303" spans="3:4" x14ac:dyDescent="0.25">
@@ -4515,7 +4515,7 @@
         <v>13</v>
       </c>
       <c r="D303" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="304" spans="3:4" x14ac:dyDescent="0.25">
@@ -4523,7 +4523,7 @@
         <v>1</v>
       </c>
       <c r="D304" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
@@ -4531,7 +4531,7 @@
         <v>48</v>
       </c>
       <c r="D305" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -4539,7 +4539,7 @@
         <v>143</v>
       </c>
       <c r="D306" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -4547,13 +4547,13 @@
         <v>97</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C307" t="s">
         <v>97</v>
       </c>
       <c r="D307" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -4561,7 +4561,7 @@
         <v>5</v>
       </c>
       <c r="D308" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4569,7 +4569,7 @@
         <v>147</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -4577,7 +4577,7 @@
         <v>146</v>
       </c>
       <c r="D310" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -4585,7 +4585,7 @@
         <v>121</v>
       </c>
       <c r="D311" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -4593,7 +4593,7 @@
         <v>2</v>
       </c>
       <c r="D312" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -4617,13 +4617,13 @@
         <v>79</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C315" t="s">
         <v>79</v>
       </c>
       <c r="D315" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4631,13 +4631,13 @@
         <v>148</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C316" t="s">
         <v>148</v>
       </c>
       <c r="D316" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
@@ -4645,7 +4645,7 @@
         <v>5</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4653,13 +4653,13 @@
         <v>85</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C318" t="s">
         <v>85</v>
       </c>
       <c r="D318" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
@@ -4667,7 +4667,7 @@
         <v>5</v>
       </c>
       <c r="D319" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -4675,7 +4675,7 @@
         <v>148</v>
       </c>
       <c r="D320" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -4683,7 +4683,7 @@
         <v>33</v>
       </c>
       <c r="D321" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4691,13 +4691,13 @@
         <v>91</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C322" t="s">
         <v>91</v>
       </c>
       <c r="D322" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
@@ -4705,7 +4705,7 @@
         <v>5</v>
       </c>
       <c r="D323" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -4721,18 +4721,18 @@
         <v>2</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C325" t="s">
         <v>2</v>
       </c>
       <c r="D325" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D325"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>